<commit_message>
Added a full functioning tab about drawdown
</commit_message>
<xml_diff>
--- a/notes/LITTLE_HISTORY_DATA.xlsx
+++ b/notes/LITTLE_HISTORY_DATA.xlsx
@@ -185,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -193,18 +193,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -500,7 +553,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -556,386 +611,394 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>39113.961111111108</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>39125.959027777775</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>39126.958333333336</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <v>39140.958333333336</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>39141.958333333336</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
         <v>39142.397916666669</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>39168.917361111111</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="2">
         <v>39171.491666666669</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>39182.916666666664</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
         <v>39206.252083333333</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>39243.750694444447</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
         <v>39243.916666666664</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>39273.916666666664</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>1328</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
         <v>39289.916666666664</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>39292.750694444447</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
         <v>39294.97152777778</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>39349.916666666664</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
         <v>39366.549305555556</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>39421.958333333336</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>1319</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>1305</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
         <v>39427.660416666666</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K2:K11">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>